<commit_message>
DDT Inter case 1020 Signed-off-by: qsy732454774 <732454774@qq.com>
</commit_message>
<xml_diff>
--- a/Cases/WebCases.xlsx
+++ b/Cases/WebCases.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D152F39-806A-40C8-A7DA-2F4AD37FA6FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF32D443-C3AE-4AEC-AA98-B329498B08B8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4950" yWindow="1050" windowWidth="23400" windowHeight="14085" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="商城后台系统用例" sheetId="2" r:id="rId1"/>
     <sheet name="商城前台系统用例" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="101">
   <si>
     <t>分组信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -334,13 +341,13 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>click</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>visitWeb</t>
   </si>
   <si>
-    <t>openBrowser</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.testingedu.com.cn:8000/Admin/Admin/login</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -416,19 +423,12 @@
   <si>
     <t>//button[contains(text(),'提交订单')]</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最大化窗口</t>
-  </si>
-  <si>
-    <t>maximize</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -445,7 +445,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -458,8 +458,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -495,11 +501,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -522,8 +541,22 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -863,22 +896,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="58.44140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="1" max="2" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="53.5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -913,7 +946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -928,9 +961,9 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="2"/>
@@ -943,9 +976,9 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
@@ -962,16 +995,18 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="9" t="s">
-        <v>101</v>
+        <v>21</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5" s="14"/>
+        <v>80</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>81</v>
+      </c>
       <c r="F5" s="10"/>
       <c r="G5" s="1"/>
       <c r="H5" s="5"/>
@@ -979,60 +1014,62 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" s="10"/>
+        <v>8</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="5"/>
+      <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>99</v>
+        <v>28</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="5"/>
@@ -1040,72 +1077,70 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="10">
-        <v>1</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F9" s="10"/>
       <c r="G9" s="1"/>
       <c r="H9" s="5"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="9" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A10" s="12"/>
+      <c r="B10" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A11" s="9"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="1"/>
@@ -1114,17 +1149,17 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="1"/>
@@ -1133,140 +1168,142 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="10"/>
+        <v>40</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="5"/>
+      <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="F15" s="10">
+        <v>52</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="9" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="10">
-        <v>52</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E16" s="10">
+        <v>1</v>
+      </c>
+      <c r="F16" s="10"/>
       <c r="G16" s="1"/>
       <c r="H16" s="5"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="9" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="10">
-        <v>1</v>
-      </c>
-      <c r="F17" s="10"/>
+        <v>43</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="10">
+        <v>54</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="5"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="9" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="10">
-        <v>54</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E18" s="10">
+        <v>1</v>
+      </c>
+      <c r="F18" s="10"/>
       <c r="G18" s="1"/>
       <c r="H18" s="5"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="9" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="10">
-        <v>1</v>
-      </c>
-      <c r="F19" s="10"/>
+        <v>43</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="10">
+        <v>374</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="5"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F20" s="10">
-        <v>374</v>
+        <v>50</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="5"/>
@@ -1274,20 +1311,20 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F21" s="10">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="5"/>
@@ -1295,38 +1332,36 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="10">
-        <v>80</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F22" s="10"/>
       <c r="G22" s="1"/>
       <c r="H22" s="5"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="1"/>
@@ -1335,41 +1370,22 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="9" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>56</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="1"/>
       <c r="H24" s="5"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1380,23 +1396,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.21875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="26.109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="60.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="60.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.75" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1431,7 +1447,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -1446,9 +1462,9 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="15" t="s">
         <v>58</v>
       </c>
       <c r="C3" s="2"/>
@@ -1461,14 +1477,14 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>60</v>
@@ -1480,56 +1496,60 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="1" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E5" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="F5" s="6"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="5"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F6" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="F6" s="6">
+        <v>13800138006</v>
+      </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="H6" s="5"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F7" s="6">
-        <v>13800138006</v>
+        <v>123456</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="5"/>
@@ -1537,20 +1557,20 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F8" s="6">
-        <v>123456</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="5"/>
@@ -1558,72 +1578,70 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="6">
-        <v>1</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="F9" s="6"/>
       <c r="G9" s="1"/>
       <c r="H9" s="5"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A10" s="2"/>
+      <c r="B10" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A11" s="1"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>97</v>
+        <v>63</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="1"/>
@@ -1632,38 +1650,36 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>8</v>
+        <v>55</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>41</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="F13" s="6"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="8" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="1"/>
@@ -1672,17 +1688,17 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="1"/>
@@ -1691,36 +1707,36 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="8" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="8" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="1"/>
@@ -1729,17 +1745,17 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="8">
-        <v>1</v>
+        <v>91</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="1"/>
@@ -1748,17 +1764,17 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="1"/>
@@ -1767,62 +1783,43 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" s="6"/>
+        <v>95</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="5"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="8" t="s">
-        <v>93</v>
+      <c r="B21" s="17"/>
+      <c r="C21" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>96</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
       <c r="G21" s="1"/>
       <c r="H21" s="5"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>